<commit_message>
Poistettiin testikooodi, ja päivitys excel-tiedostoon
</commit_message>
<xml_diff>
--- a/documentation/hashtable_collision_tests/random_permutations_collisions.xlsx
+++ b/documentation/hashtable_collision_tests/random_permutations_collisions.xlsx
@@ -47,17 +47,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -117,7 +117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -135,10 +135,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -162,14 +158,14 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="2" width="15.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="2" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -620,15 +616,15 @@
         <f aca="false">AVERAGE(B2:B21)</f>
         <v>7.4</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" s="4" t="n">
         <f aca="false">AVERAGE(C2:C21)</f>
         <v>1000000</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="D22" s="4" t="n">
         <f aca="false">AVERAGE(D2:D21)</f>
         <v>740081.15</v>
       </c>
-      <c r="E22" s="5" t="n">
+      <c r="E22" s="4" t="n">
         <f aca="false">AVERAGE(E2:E21)</f>
         <v>832787.85</v>
       </c>

</xml_diff>